<commit_message>
Changed data example file
</commit_message>
<xml_diff>
--- a/data/phospho_human.xlsx
+++ b/data/phospho_human.xlsx
@@ -3110,33 +3110,32 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+      <selection pane="topLeft" activeCell="C201" activeCellId="0" sqref="A1:C201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.46"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>